<commit_message>
RadioButton i WebTables Pages
Dodala RadioButtonPage i WebTablesPages
</commit_message>
<xml_diff>
--- a/TextBook.xlsx
+++ b/TextBook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7515"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="URL" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>https://demoqa.com/</t>
   </si>
@@ -83,6 +83,24 @@
   </si>
   <si>
     <t>https://demoqa.com/checkbox</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>RadioButtonPage URL</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/radio-button</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>https://demoqa.com/webtables</t>
+  </si>
+  <si>
+    <t>WebTablesPage URL</t>
   </si>
 </sst>
 </file>
@@ -412,17 +430,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -479,6 +497,28 @@
       </c>
       <c r="C5" s="1" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>